<commit_message>
Removed redundant information and corrected typo
</commit_message>
<xml_diff>
--- a/additional_materials/code-stats/linesAndFilesCount.xlsx
+++ b/additional_materials/code-stats/linesAndFilesCount.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfichen\Amaya-Workbench\additional_materials\code-stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1A76FE-E049-423D-A013-B336404F4655}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCB85AB-D61F-42DB-BA08-BE4A44174344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6060" activeTab="1" xr2:uid="{E9240D72-A473-4962-A29C-2FDF22575481}"/>
   </bookViews>
@@ -169,10 +169,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.2565805690189199"/>
-          <c:y val="0.10743061772605192"/>
-          <c:w val="0.55062651921171091"/>
-          <c:h val="0.62343679287179521"/>
+          <c:x val="0.22385108378874696"/>
+          <c:y val="0.16442977737590009"/>
+          <c:w val="0.58335597515952364"/>
+          <c:h val="0.56643755238893545"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -475,8 +475,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.76167656876328149"/>
-              <c:y val="1.4430949040949111E-2"/>
+              <c:x val="0.75228709941147509"/>
+              <c:y val="5.4107366414358878E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -687,8 +687,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="7.9835321148413116E-2"/>
-              <c:y val="1.0354224969864444E-2"/>
+              <c:x val="0.14679271295359936"/>
+              <c:y val="5.0812875242672369E-2"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -750,6 +750,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.36871933548654501"/>
+          <c:y val="0.88978125430768096"/>
+          <c:w val="0.24253457422663963"/>
+          <c:h val="4.0419414083142757E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1416,16 +1426,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>711199</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
+      <xdr:colOff>444502</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:rowOff>28579</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1804,7 +1814,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>